<commit_message>
tests working, enum symptom, file.drl fixed etc etc
</commit_message>
<xml_diff>
--- a/src/main/resources/symptom_weights/Symptoms_DSS.xlsx
+++ b/src/main/resources/symptom_weights/Symptoms_DSS.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27518"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{724B4091-5AD9-4F50-B5BA-1C958165173A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elenamacarron/Desktop/pruebaDSS/NeuroDD/src/main/resources/symptom_weights/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F442C9-B649-3B43-B3E6-CF079C2491C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="14800" windowHeight="8020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Desicion Matrix" sheetId="5" r:id="rId1"/>
@@ -365,9 +370,6 @@
     <t>orientation impairment</t>
   </si>
   <si>
-    <t>scanning  speech</t>
-  </si>
-  <si>
     <t>social isolation</t>
   </si>
   <si>
@@ -474,13 +476,16 @@
   </si>
   <si>
     <t>PREVIOUS TABLE, NOW WE PUT SCORES</t>
+  </si>
+  <si>
+    <t>scanning speech</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,7 +497,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -635,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -747,9 +752,6 @@
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,9 +779,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -817,7 +819,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -923,7 +925,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1065,7 +1067,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1079,35 +1081,35 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" customWidth="1"/>
+    <col min="12" max="12" width="10.5" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" customWidth="1"/>
-    <col min="26" max="26" width="10.140625" customWidth="1"/>
-    <col min="27" max="27" width="13.28515625" customWidth="1"/>
-    <col min="28" max="28" width="10.5703125" customWidth="1"/>
-    <col min="30" max="30" width="10.85546875" customWidth="1"/>
-    <col min="31" max="31" width="12.140625" customWidth="1"/>
-    <col min="34" max="34" width="12.7109375" customWidth="1"/>
-    <col min="35" max="35" width="11.7109375" customWidth="1"/>
-    <col min="37" max="37" width="10.85546875" customWidth="1"/>
-    <col min="38" max="38" width="11.140625" customWidth="1"/>
-    <col min="39" max="39" width="12.42578125" customWidth="1"/>
-    <col min="40" max="40" width="13.28515625" customWidth="1"/>
-    <col min="43" max="43" width="11.42578125" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" customWidth="1"/>
+    <col min="26" max="26" width="10.1640625" customWidth="1"/>
+    <col min="27" max="27" width="13.33203125" customWidth="1"/>
+    <col min="28" max="28" width="10.5" customWidth="1"/>
+    <col min="30" max="30" width="10.83203125" customWidth="1"/>
+    <col min="31" max="31" width="12.1640625" customWidth="1"/>
+    <col min="34" max="34" width="12.6640625" customWidth="1"/>
+    <col min="35" max="35" width="11.6640625" customWidth="1"/>
+    <col min="37" max="37" width="10.83203125" customWidth="1"/>
+    <col min="38" max="38" width="11.1640625" customWidth="1"/>
+    <col min="39" max="39" width="12.5" customWidth="1"/>
+    <col min="40" max="40" width="13.33203125" customWidth="1"/>
+    <col min="43" max="43" width="11.5" customWidth="1"/>
     <col min="45" max="45" width="12" customWidth="1"/>
-    <col min="47" max="48" width="13.28515625" customWidth="1"/>
+    <col min="47" max="48" width="13.33203125" customWidth="1"/>
     <col min="51" max="51" width="12" customWidth="1"/>
-    <col min="55" max="55" width="12.85546875" customWidth="1"/>
+    <col min="55" max="55" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="35" t="s">
         <v>0</v>
@@ -1172,7 +1174,7 @@
       <c r="BB1" s="38"/>
       <c r="BC1" s="38"/>
     </row>
-    <row r="2" spans="1:55" ht="76.5">
+    <row r="2" spans="1:55" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1339,7 +1341,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:55" s="2" customFormat="1">
+    <row r="3" spans="1:55" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
         <v>59</v>
       </c>
@@ -1506,7 +1508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:55" s="2" customFormat="1">
+    <row r="4" spans="1:55" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>62</v>
       </c>
@@ -1673,7 +1675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:55" s="2" customFormat="1">
+    <row r="5" spans="1:55" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>63</v>
       </c>
@@ -1840,7 +1842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:55" s="2" customFormat="1">
+    <row r="6" spans="1:55" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
         <v>64</v>
       </c>
@@ -2007,7 +2009,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:55" s="2" customFormat="1">
+    <row r="7" spans="1:55" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
         <v>65</v>
       </c>
@@ -2174,7 +2176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:55" s="2" customFormat="1">
+    <row r="8" spans="1:55" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
         <v>66</v>
       </c>
@@ -2341,7 +2343,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:55">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.2">
       <c r="T9" s="1"/>
       <c r="AL9" s="4"/>
       <c r="AS9" s="1"/>
@@ -2350,7 +2352,7 @@
       <c r="AV9" s="1"/>
       <c r="AX9" s="1"/>
     </row>
-    <row r="10" spans="1:55">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.2">
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
       <c r="D10" s="34"/>
@@ -2377,7 +2379,7 @@
       <c r="AX10" s="1"/>
       <c r="BC10" s="34"/>
     </row>
-    <row r="11" spans="1:55">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2387,7 +2389,7 @@
       <c r="G11" s="2"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:55">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2396,7 +2398,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:55">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -2407,7 +2409,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:55">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>68</v>
       </c>
@@ -2426,7 +2428,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:55">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>69</v>
       </c>
@@ -2452,7 +2454,7 @@
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
     </row>
-    <row r="16" spans="1:55">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>70</v>
       </c>
@@ -2478,7 +2480,7 @@
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>71</v>
       </c>
@@ -2504,7 +2506,7 @@
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>72</v>
       </c>
@@ -2530,7 +2532,7 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>73</v>
       </c>
@@ -2556,7 +2558,7 @@
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2580,7 +2582,7 @@
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -2598,7 +2600,7 @@
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -2616,7 +2618,7 @@
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -2634,7 +2636,7 @@
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -2652,7 +2654,7 @@
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -2672,7 +2674,7 @@
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>75</v>
       </c>
@@ -2694,7 +2696,7 @@
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -2714,7 +2716,7 @@
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2738,7 +2740,7 @@
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
     </row>
-    <row r="29" spans="1:22" ht="30.75">
+    <row r="29" spans="1:22" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="14"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2764,7 +2766,7 @@
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="14"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2788,7 +2790,7 @@
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2812,7 +2814,7 @@
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
     </row>
-    <row r="32" spans="1:22">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2836,7 +2838,7 @@
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
     </row>
-    <row r="33" spans="1:76">
+    <row r="33" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A33" s="14"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2860,7 +2862,7 @@
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
     </row>
-    <row r="34" spans="1:76">
+    <row r="34" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2884,7 +2886,7 @@
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
     </row>
-    <row r="35" spans="1:76">
+    <row r="35" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2908,7 +2910,7 @@
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
     </row>
-    <row r="36" spans="1:76">
+    <row r="36" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2932,7 +2934,7 @@
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
     </row>
-    <row r="37" spans="1:76">
+    <row r="37" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2956,7 +2958,7 @@
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
     </row>
-    <row r="38" spans="1:76">
+    <row r="38" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2980,7 +2982,7 @@
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
     </row>
-    <row r="39" spans="1:76">
+    <row r="39" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -3004,7 +3006,7 @@
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
     </row>
-    <row r="40" spans="1:76">
+    <row r="40" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -3028,7 +3030,7 @@
       <c r="U40" s="2"/>
       <c r="V40" s="2"/>
     </row>
-    <row r="41" spans="1:76">
+    <row r="41" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -3052,7 +3054,7 @@
       <c r="U41" s="2"/>
       <c r="V41" s="2"/>
     </row>
-    <row r="42" spans="1:76">
+    <row r="42" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -3076,7 +3078,7 @@
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
     </row>
-    <row r="43" spans="1:76">
+    <row r="43" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -3100,7 +3102,7 @@
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
     </row>
-    <row r="44" spans="1:76">
+    <row r="44" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -3124,7 +3126,7 @@
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
     </row>
-    <row r="45" spans="1:76">
+    <row r="45" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -3202,7 +3204,7 @@
       <c r="BW45" s="2"/>
       <c r="BX45" s="2"/>
     </row>
-    <row r="46" spans="1:76">
+    <row r="46" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -3280,7 +3282,7 @@
       <c r="BW46" s="2"/>
       <c r="BX46" s="2"/>
     </row>
-    <row r="47" spans="1:76">
+    <row r="47" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -3358,7 +3360,7 @@
       <c r="BW47" s="2"/>
       <c r="BX47" s="2"/>
     </row>
-    <row r="48" spans="1:76">
+    <row r="48" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A48" s="14"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -3436,7 +3438,7 @@
       <c r="BW48" s="2"/>
       <c r="BX48" s="2"/>
     </row>
-    <row r="49" spans="1:76">
+    <row r="49" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -3514,7 +3516,7 @@
       <c r="BW49" s="2"/>
       <c r="BX49" s="2"/>
     </row>
-    <row r="50" spans="1:76">
+    <row r="50" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -3592,7 +3594,7 @@
       <c r="BW50" s="2"/>
       <c r="BX50" s="2"/>
     </row>
-    <row r="51" spans="1:76">
+    <row r="51" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -3670,7 +3672,7 @@
       <c r="BW51" s="2"/>
       <c r="BX51" s="2"/>
     </row>
-    <row r="52" spans="1:76">
+    <row r="52" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -3748,7 +3750,7 @@
       <c r="BW52" s="2"/>
       <c r="BX52" s="2"/>
     </row>
-    <row r="53" spans="1:76">
+    <row r="53" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -3826,7 +3828,7 @@
       <c r="BW53" s="2"/>
       <c r="BX53" s="2"/>
     </row>
-    <row r="54" spans="1:76">
+    <row r="54" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -3904,7 +3906,7 @@
       <c r="BW54" s="2"/>
       <c r="BX54" s="2"/>
     </row>
-    <row r="55" spans="1:76">
+    <row r="55" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -3982,7 +3984,7 @@
       <c r="BW55" s="2"/>
       <c r="BX55" s="2"/>
     </row>
-    <row r="56" spans="1:76">
+    <row r="56" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -4060,7 +4062,7 @@
       <c r="BW56" s="2"/>
       <c r="BX56" s="2"/>
     </row>
-    <row r="57" spans="1:76">
+    <row r="57" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -4138,7 +4140,7 @@
       <c r="BW57" s="2"/>
       <c r="BX57" s="2"/>
     </row>
-    <row r="58" spans="1:76">
+    <row r="58" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -4216,7 +4218,7 @@
       <c r="BW58" s="2"/>
       <c r="BX58" s="2"/>
     </row>
-    <row r="59" spans="1:76">
+    <row r="59" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -4294,7 +4296,7 @@
       <c r="BW59" s="2"/>
       <c r="BX59" s="2"/>
     </row>
-    <row r="60" spans="1:76">
+    <row r="60" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -4372,7 +4374,7 @@
       <c r="BW60" s="2"/>
       <c r="BX60" s="2"/>
     </row>
-    <row r="61" spans="1:76">
+    <row r="61" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -4450,7 +4452,7 @@
       <c r="BW61" s="2"/>
       <c r="BX61" s="2"/>
     </row>
-    <row r="62" spans="1:76">
+    <row r="62" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -4528,7 +4530,7 @@
       <c r="BW62" s="2"/>
       <c r="BX62" s="2"/>
     </row>
-    <row r="63" spans="1:76">
+    <row r="63" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -4606,7 +4608,7 @@
       <c r="BW63" s="2"/>
       <c r="BX63" s="2"/>
     </row>
-    <row r="64" spans="1:76">
+    <row r="64" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -4684,7 +4686,7 @@
       <c r="BW64" s="2"/>
       <c r="BX64" s="2"/>
     </row>
-    <row r="65" spans="58:76">
+    <row r="65" spans="58:76" x14ac:dyDescent="0.2">
       <c r="BF65" s="2"/>
       <c r="BG65" s="2"/>
       <c r="BH65" s="2"/>
@@ -4705,7 +4707,7 @@
       <c r="BW65" s="2"/>
       <c r="BX65" s="2"/>
     </row>
-    <row r="66" spans="58:76">
+    <row r="66" spans="58:76" x14ac:dyDescent="0.2">
       <c r="BF66" s="2"/>
       <c r="BG66" s="2"/>
       <c r="BH66" s="2"/>
@@ -4726,7 +4728,7 @@
       <c r="BW66" s="2"/>
       <c r="BX66" s="2"/>
     </row>
-    <row r="67" spans="58:76">
+    <row r="67" spans="58:76" x14ac:dyDescent="0.2">
       <c r="BF67" s="2"/>
       <c r="BG67" s="2"/>
       <c r="BH67" s="2"/>
@@ -4747,7 +4749,7 @@
       <c r="BW67" s="2"/>
       <c r="BX67" s="2"/>
     </row>
-    <row r="68" spans="58:76">
+    <row r="68" spans="58:76" x14ac:dyDescent="0.2">
       <c r="BF68" s="2"/>
       <c r="BG68" s="2"/>
       <c r="BH68" s="2"/>
@@ -4768,7 +4770,7 @@
       <c r="BW68" s="2"/>
       <c r="BX68" s="2"/>
     </row>
-    <row r="69" spans="58:76">
+    <row r="69" spans="58:76" x14ac:dyDescent="0.2">
       <c r="BF69" s="2"/>
       <c r="BG69" s="2"/>
       <c r="BH69" s="2"/>
@@ -4789,7 +4791,7 @@
       <c r="BW69" s="2"/>
       <c r="BX69" s="2"/>
     </row>
-    <row r="70" spans="58:76">
+    <row r="70" spans="58:76" x14ac:dyDescent="0.2">
       <c r="BF70" s="2"/>
       <c r="BG70" s="2"/>
       <c r="BH70" s="2"/>
@@ -4810,7 +4812,7 @@
       <c r="BW70" s="2"/>
       <c r="BX70" s="2"/>
     </row>
-    <row r="71" spans="58:76">
+    <row r="71" spans="58:76" x14ac:dyDescent="0.2">
       <c r="BF71" s="2"/>
       <c r="BG71" s="2"/>
       <c r="BH71" s="2"/>
@@ -4831,7 +4833,7 @@
       <c r="BW71" s="2"/>
       <c r="BX71" s="2"/>
     </row>
-    <row r="72" spans="58:76">
+    <row r="72" spans="58:76" x14ac:dyDescent="0.2">
       <c r="BF72" s="2"/>
       <c r="BG72" s="2"/>
       <c r="BH72" s="2"/>
@@ -4867,31 +4869,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D73EA267-64A2-42BE-BF3E-54987D18375A}">
   <dimension ref="A2:BB9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" customWidth="1"/>
-    <col min="16" max="16" width="17.140625" customWidth="1"/>
-    <col min="19" max="19" width="15.28515625" customWidth="1"/>
-    <col min="26" max="26" width="16.7109375" customWidth="1"/>
-    <col min="31" max="31" width="17.85546875" customWidth="1"/>
-    <col min="35" max="35" width="16.42578125" customWidth="1"/>
-    <col min="37" max="37" width="16.42578125" customWidth="1"/>
-    <col min="38" max="38" width="14.5703125" customWidth="1"/>
+    <col min="13" max="13" width="17.5" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" customWidth="1"/>
+    <col min="16" max="16" width="17.1640625" customWidth="1"/>
+    <col min="19" max="19" width="15.33203125" customWidth="1"/>
+    <col min="26" max="26" width="16.6640625" customWidth="1"/>
+    <col min="31" max="31" width="17.83203125" customWidth="1"/>
+    <col min="35" max="35" width="16.5" customWidth="1"/>
+    <col min="37" max="37" width="16.5" customWidth="1"/>
+    <col min="38" max="38" width="14.5" customWidth="1"/>
     <col min="50" max="50" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:54">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="35" t="s">
         <v>0</v>
@@ -4955,7 +4957,7 @@
       <c r="BA2" s="38"/>
       <c r="BB2" s="38"/>
     </row>
-    <row r="3" spans="1:54" ht="76.5">
+    <row r="3" spans="1:54" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -4971,10 +4973,10 @@
       <c r="E3" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="9" t="s">
         <v>84</v>
       </c>
       <c r="H3" s="8" t="s">
@@ -5007,13 +5009,13 @@
       <c r="Q3" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="R3" s="39" t="s">
+      <c r="R3" s="9" t="s">
         <v>95</v>
       </c>
       <c r="S3" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="T3" s="39" t="s">
+      <c r="T3" s="9" t="s">
         <v>97</v>
       </c>
       <c r="U3" s="8" t="s">
@@ -5034,7 +5036,7 @@
       <c r="Z3" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AA3" s="39" t="s">
+      <c r="AA3" s="9" t="s">
         <v>104</v>
       </c>
       <c r="AB3" s="8" t="s">
@@ -5043,83 +5045,83 @@
       <c r="AC3" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="AD3" s="39" t="s">
+      <c r="AD3" s="9" t="s">
         <v>107</v>
       </c>
       <c r="AE3" s="8" t="s">
         <v>108</v>
       </c>
       <c r="AF3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG3" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="AG3" s="8" t="s">
+      <c r="AH3" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="AH3" s="8" t="s">
+      <c r="AI3" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="AI3" s="8" t="s">
+      <c r="AJ3" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="AJ3" s="8" t="s">
+      <c r="AK3" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="AK3" s="8" t="s">
+      <c r="AL3" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="AL3" s="8" t="s">
+      <c r="AM3" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="AM3" s="8" t="s">
+      <c r="AN3" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="AN3" s="8" t="s">
+      <c r="AO3" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="AO3" s="8" t="s">
+      <c r="AP3" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="AP3" s="8" t="s">
+      <c r="AQ3" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="AQ3" s="8" t="s">
+      <c r="AR3" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="AR3" s="8" t="s">
+      <c r="AS3" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="AS3" s="39" t="s">
+      <c r="AT3" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="AT3" s="8" t="s">
+      <c r="AU3" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="AU3" s="8" t="s">
+      <c r="AV3" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="AV3" s="8" t="s">
+      <c r="AW3" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="AW3" s="39" t="s">
+      <c r="AX3" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="AX3" s="8" t="s">
+      <c r="AY3" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="AY3" s="8" t="s">
+      <c r="AZ3" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="AZ3" s="8" t="s">
+      <c r="BA3" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="BA3" s="8" t="s">
+      <c r="BB3" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="BB3" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:54">
+    </row>
+    <row r="4" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>59</v>
       </c>
@@ -5283,7 +5285,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:54">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>62</v>
       </c>
@@ -5447,9 +5449,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:54">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" s="4">
         <v>4</v>
@@ -5611,7 +5613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:54">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
         <v>64</v>
       </c>
@@ -5775,7 +5777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:54">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
         <v>65</v>
       </c>
@@ -5939,7 +5941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:54">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
         <v>66</v>
       </c>
@@ -6122,13 +6124,13 @@
       <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="35" t="s">
         <v>0</v>
@@ -6166,24 +6168,24 @@
       <c r="AA2" s="38"/>
       <c r="AB2" s="38"/>
     </row>
-    <row r="3" spans="1:28" ht="91.5">
+    <row r="3" spans="1:28" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>13</v>
@@ -6252,7 +6254,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>59</v>
       </c>
@@ -6304,7 +6306,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>62</v>
       </c>
@@ -6352,7 +6354,7 @@
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
         <v>63</v>
       </c>
@@ -6394,7 +6396,7 @@
       <c r="AA6" s="4"/>
       <c r="AB6" s="4"/>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
         <v>64</v>
       </c>
@@ -6438,7 +6440,7 @@
       <c r="AA7" s="4"/>
       <c r="AB7" s="4"/>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
         <v>65</v>
       </c>
@@ -6482,7 +6484,7 @@
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
         <v>66</v>
       </c>
@@ -6545,39 +6547,39 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="10.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" style="1"/>
+    <col min="10" max="10" width="10.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" style="1" customWidth="1"/>
     <col min="15" max="15" width="12" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="1"/>
+    <col min="16" max="16" width="9.1640625" style="1"/>
     <col min="17" max="17" width="8" style="1" customWidth="1"/>
-    <col min="18" max="18" width="11.28515625" style="1" customWidth="1"/>
-    <col min="19" max="45" width="9.140625" style="1"/>
-    <col min="46" max="46" width="13.140625" style="1" customWidth="1"/>
-    <col min="47" max="55" width="9.140625" style="1"/>
-    <col min="56" max="56" width="12.28515625" style="1" customWidth="1"/>
-    <col min="57" max="16384" width="9.140625" style="1"/>
+    <col min="18" max="18" width="11.33203125" style="1" customWidth="1"/>
+    <col min="19" max="45" width="9.1640625" style="1"/>
+    <col min="46" max="46" width="13.1640625" style="1" customWidth="1"/>
+    <col min="47" max="55" width="9.1640625" style="1"/>
+    <col min="56" max="56" width="12.33203125" style="1" customWidth="1"/>
+    <col min="57" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57">
+    <row r="1" spans="1:57" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="2" spans="1:57" ht="91.5">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:57" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -6624,7 +6626,7 @@
         <v>7</v>
       </c>
       <c r="P2" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q2" s="26" t="s">
         <v>41</v>
@@ -6642,7 +6644,7 @@
         <v>43</v>
       </c>
       <c r="V2" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="W2" s="27" t="s">
         <v>50</v>
@@ -6705,7 +6707,7 @@
         <v>13</v>
       </c>
       <c r="AQ2" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AR2" s="26" t="s">
         <v>45</v>
@@ -6744,326 +6746,326 @@
         <v>58</v>
       </c>
       <c r="BD2" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="BE2" s="26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:57">
+    <row r="3" spans="1:57" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z3" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AF3" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AH3" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AJ3" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AM3" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AW3" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:57">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:57" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>62</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z4" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AC4" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AF4" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AG4" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI4" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AJ4" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AK4" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AW4" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AY4" s="4"/>
       <c r="BA4" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BC4" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BE4" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:57">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:57" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AD5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AH5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AJ5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AR5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AV5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AX5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AY5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BA5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BB5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BD5" s="4"/>
       <c r="BE5" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:57">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:57" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AA6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AB6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AE6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AH6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AJ6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AK6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AL6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AO6" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AP6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AQ6" s="4"/>
       <c r="AU6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AY6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BA6" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BB6" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BC6" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:57">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:57" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>65</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AC7" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AK7" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AQ7" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AT7" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:57">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:57" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>144</v>
-      </c>
       <c r="Y8" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AJ8" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AN8" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AS8" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AZ8" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BA8" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BB8" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -7079,17 +7081,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:42" ht="76.5">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -7157,7 +7159,7 @@
         <v>28</v>
       </c>
       <c r="W2" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X2" s="9" t="s">
         <v>30</v>
@@ -7181,7 +7183,7 @@
         <v>36</v>
       </c>
       <c r="AE2" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AF2" s="8" t="s">
         <v>37</v>
@@ -7217,12 +7219,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:42">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -7230,59 +7232,59 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:42">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>63</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:42">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:42">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>64</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:42">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>65</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:42">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>63</v>
       </c>
@@ -7290,12 +7292,12 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:42">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>62</v>
       </c>
@@ -7304,7 +7306,7 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -7320,7 +7322,7 @@
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
     </row>
-    <row r="10" spans="1:42">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>64</v>
       </c>
@@ -7329,7 +7331,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -7345,7 +7347,7 @@
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
     </row>
-    <row r="11" spans="1:42">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>59</v>
       </c>
@@ -7355,7 +7357,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -7370,7 +7372,7 @@
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
     </row>
-    <row r="12" spans="1:42">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>62</v>
       </c>
@@ -7380,7 +7382,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -7395,7 +7397,7 @@
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:42">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>63</v>
       </c>
@@ -7405,7 +7407,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -7420,7 +7422,7 @@
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
     </row>
-    <row r="14" spans="1:42">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>64</v>
       </c>
@@ -7430,7 +7432,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -7445,7 +7447,7 @@
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
     </row>
-    <row r="15" spans="1:42">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>66</v>
       </c>
@@ -7455,7 +7457,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -7470,12 +7472,12 @@
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
     </row>
-    <row r="16" spans="1:42">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>62</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -7489,12 +7491,12 @@
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>64</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -7508,12 +7510,12 @@
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
         <v>65</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -7527,13 +7529,13 @@
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>66</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -7546,14 +7548,14 @@
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>64</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -7565,7 +7567,7 @@
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
         <v>66</v>
       </c>
@@ -7573,7 +7575,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -7584,7 +7586,7 @@
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
         <v>62</v>
       </c>
@@ -7593,7 +7595,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -7603,7 +7605,7 @@
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
         <v>63</v>
       </c>
@@ -7618,7 +7620,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -7628,7 +7630,7 @@
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
         <v>65</v>
       </c>
@@ -7643,7 +7645,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -7653,7 +7655,7 @@
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
         <v>65</v>
       </c>
@@ -7669,7 +7671,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -7678,7 +7680,7 @@
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
         <v>66</v>
       </c>
@@ -7694,7 +7696,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -7703,7 +7705,7 @@
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
         <v>62</v>
       </c>
@@ -7720,7 +7722,7 @@
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
@@ -7728,7 +7730,7 @@
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
         <v>65</v>
       </c>
@@ -7745,7 +7747,7 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
@@ -7753,7 +7755,7 @@
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
         <v>59</v>
       </c>
@@ -7771,14 +7773,14 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
         <v>62</v>
       </c>
@@ -7796,14 +7798,14 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>64</v>
       </c>
@@ -7822,13 +7824,13 @@
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
       <c r="P31" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
         <v>63</v>
       </c>
@@ -7848,12 +7850,12 @@
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R32" s="2"/>
       <c r="S32" s="2"/>
     </row>
-    <row r="33" spans="1:33">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>64</v>
       </c>
@@ -7873,12 +7875,12 @@
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
       <c r="Q33" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
     </row>
-    <row r="34" spans="1:33">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
         <v>66</v>
       </c>
@@ -7898,12 +7900,12 @@
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
       <c r="Q34" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
     </row>
-    <row r="35" spans="1:33">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
         <v>62</v>
       </c>
@@ -7924,11 +7926,11 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="S35" s="2"/>
     </row>
-    <row r="36" spans="1:33">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
         <v>63</v>
       </c>
@@ -7949,11 +7951,11 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="S36" s="2"/>
     </row>
-    <row r="37" spans="1:33">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>64</v>
       </c>
@@ -7974,11 +7976,11 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
       <c r="R37" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="S37" s="2"/>
     </row>
-    <row r="38" spans="1:33">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="s">
         <v>66</v>
       </c>
@@ -7999,11 +8001,11 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
       <c r="R38" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="S38" s="2"/>
     </row>
-    <row r="39" spans="1:33">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="s">
         <v>66</v>
       </c>
@@ -8025,10 +8027,10 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
       <c r="S39" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="40" spans="1:33">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
         <v>59</v>
       </c>
@@ -8051,7 +8053,7 @@
       <c r="R40" s="2"/>
       <c r="S40" s="2"/>
       <c r="T40" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="U40" s="2"/>
       <c r="V40" s="2"/>
@@ -8067,7 +8069,7 @@
       <c r="AF40" s="2"/>
       <c r="AG40" s="2"/>
     </row>
-    <row r="41" spans="1:33">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A41" s="18" t="s">
         <v>62</v>
       </c>
@@ -8090,7 +8092,7 @@
       <c r="R41" s="2"/>
       <c r="S41" s="2"/>
       <c r="T41" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="U41" s="2"/>
       <c r="V41" s="2"/>
@@ -8106,7 +8108,7 @@
       <c r="AF41" s="2"/>
       <c r="AG41" s="2"/>
     </row>
-    <row r="42" spans="1:33">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
         <v>63</v>
       </c>
@@ -8129,7 +8131,7 @@
       <c r="R42" s="2"/>
       <c r="S42" s="2"/>
       <c r="T42" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
@@ -8145,7 +8147,7 @@
       <c r="AF42" s="2"/>
       <c r="AG42" s="2"/>
     </row>
-    <row r="43" spans="1:33">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
         <v>65</v>
       </c>
@@ -8168,7 +8170,7 @@
       <c r="R43" s="2"/>
       <c r="S43" s="2"/>
       <c r="T43" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
@@ -8184,7 +8186,7 @@
       <c r="AF43" s="2"/>
       <c r="AG43" s="2"/>
     </row>
-    <row r="44" spans="1:33">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A44" s="16" t="s">
         <v>66</v>
       </c>
@@ -8207,7 +8209,7 @@
       <c r="R44" s="2"/>
       <c r="S44" s="2"/>
       <c r="T44" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
@@ -8223,7 +8225,7 @@
       <c r="AF44" s="2"/>
       <c r="AG44" s="2"/>
     </row>
-    <row r="45" spans="1:33">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
         <v>59</v>
       </c>
@@ -8247,7 +8249,7 @@
       <c r="S45" s="2"/>
       <c r="T45" s="2"/>
       <c r="U45" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="V45" s="2"/>
       <c r="W45" s="2"/>
@@ -8262,7 +8264,7 @@
       <c r="AF45" s="2"/>
       <c r="AG45" s="2"/>
     </row>
-    <row r="46" spans="1:33">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
         <v>63</v>
       </c>
@@ -8286,7 +8288,7 @@
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
       <c r="U46" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="V46" s="2"/>
       <c r="W46" s="2"/>
@@ -8301,7 +8303,7 @@
       <c r="AF46" s="2"/>
       <c r="AG46" s="2"/>
     </row>
-    <row r="47" spans="1:33">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
         <v>63</v>
       </c>
@@ -8326,7 +8328,7 @@
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
       <c r="V47" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="W47" s="2"/>
       <c r="X47" s="2"/>
@@ -8340,7 +8342,7 @@
       <c r="AF47" s="2"/>
       <c r="AG47" s="2"/>
     </row>
-    <row r="48" spans="1:33">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
         <v>64</v>
       </c>
@@ -8365,7 +8367,7 @@
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
       <c r="V48" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="W48" s="2"/>
       <c r="X48" s="2"/>
@@ -8379,7 +8381,7 @@
       <c r="AF48" s="2"/>
       <c r="AG48" s="2"/>
     </row>
-    <row r="49" spans="1:33">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
         <v>63</v>
       </c>
@@ -8405,7 +8407,7 @@
       <c r="U49" s="2"/>
       <c r="V49" s="2"/>
       <c r="W49" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="X49" s="2"/>
       <c r="Y49" s="2"/>
@@ -8418,7 +8420,7 @@
       <c r="AF49" s="2"/>
       <c r="AG49" s="2"/>
     </row>
-    <row r="50" spans="1:33">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
         <v>59</v>
       </c>
@@ -8445,7 +8447,7 @@
       <c r="V50" s="2"/>
       <c r="W50" s="2"/>
       <c r="X50" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Y50" s="2"/>
       <c r="Z50" s="2"/>
@@ -8457,7 +8459,7 @@
       <c r="AF50" s="2"/>
       <c r="AG50" s="2"/>
     </row>
-    <row r="51" spans="1:33">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A51" s="18" t="s">
         <v>62</v>
       </c>
@@ -8484,7 +8486,7 @@
       <c r="V51" s="2"/>
       <c r="W51" s="2"/>
       <c r="X51" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Y51" s="2"/>
       <c r="Z51" s="2"/>
@@ -8496,7 +8498,7 @@
       <c r="AF51" s="2"/>
       <c r="AG51" s="2"/>
     </row>
-    <row r="52" spans="1:33">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
         <v>64</v>
       </c>
@@ -8524,7 +8526,7 @@
       <c r="W52" s="2"/>
       <c r="X52" s="2"/>
       <c r="Y52" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z52" s="2"/>
       <c r="AA52" s="2"/>
@@ -8535,7 +8537,7 @@
       <c r="AF52" s="2"/>
       <c r="AG52" s="2"/>
     </row>
-    <row r="53" spans="1:33">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>64</v>
       </c>
@@ -8564,7 +8566,7 @@
       <c r="X53" s="2"/>
       <c r="Y53" s="2"/>
       <c r="Z53" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AA53" s="2"/>
       <c r="AB53" s="2"/>
@@ -8574,7 +8576,7 @@
       <c r="AF53" s="2"/>
       <c r="AG53" s="2"/>
     </row>
-    <row r="54" spans="1:33">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
         <v>59</v>
       </c>
@@ -8604,7 +8606,7 @@
       <c r="Y54" s="2"/>
       <c r="Z54" s="2"/>
       <c r="AA54" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AB54" s="2"/>
       <c r="AC54" s="2"/>
@@ -8613,7 +8615,7 @@
       <c r="AF54" s="2"/>
       <c r="AG54" s="2"/>
     </row>
-    <row r="55" spans="1:33">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
         <v>63</v>
       </c>
@@ -8643,7 +8645,7 @@
       <c r="Y55" s="2"/>
       <c r="Z55" s="2"/>
       <c r="AA55" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AB55" s="2"/>
       <c r="AC55" s="2"/>
@@ -8652,7 +8654,7 @@
       <c r="AF55" s="2"/>
       <c r="AG55" s="2"/>
     </row>
-    <row r="56" spans="1:33">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A56" s="17" t="s">
         <v>64</v>
       </c>
@@ -8682,7 +8684,7 @@
       <c r="Y56" s="2"/>
       <c r="Z56" s="2"/>
       <c r="AA56" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AB56" s="2"/>
       <c r="AC56" s="2"/>
@@ -8691,7 +8693,7 @@
       <c r="AF56" s="2"/>
       <c r="AG56" s="2"/>
     </row>
-    <row r="57" spans="1:33">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A57" s="20" t="s">
         <v>59</v>
       </c>
@@ -8722,7 +8724,7 @@
       <c r="Z57" s="2"/>
       <c r="AA57" s="2"/>
       <c r="AB57" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AC57" s="2"/>
       <c r="AD57" s="2"/>
@@ -8730,7 +8732,7 @@
       <c r="AF57" s="2"/>
       <c r="AG57" s="2"/>
     </row>
-    <row r="58" spans="1:33">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A58" s="17" t="s">
         <v>64</v>
       </c>
@@ -8762,14 +8764,14 @@
       <c r="AA58" s="2"/>
       <c r="AB58" s="2"/>
       <c r="AC58" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AD58" s="2"/>
       <c r="AE58" s="2"/>
       <c r="AF58" s="2"/>
       <c r="AG58" s="2"/>
     </row>
-    <row r="59" spans="1:33">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
         <v>63</v>
       </c>
@@ -8802,7 +8804,7 @@
       <c r="AB59" s="2"/>
       <c r="AC59" s="2"/>
       <c r="AD59" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AE59" s="2"/>
       <c r="AF59" s="2"/>

</xml_diff>